<commit_message>
Further edits, table updates -Discarding old .tex files.
</commit_message>
<xml_diff>
--- a/results/bias_tests.xlsx
+++ b/results/bias_tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhilgard\Documents\GitHub\craig_meta\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhilgard.APP401B-2-U2\Documents\GitHub\craig_meta\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
   <si>
     <t>Outcome</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>p_{p-uniform}</t>
-  </si>
-  <si>
-    <t>p_{TES}</t>
   </si>
   <si>
     <t>Beta_{Egger}</t>
@@ -75,7 +72,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=".000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -553,9 +553,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -877,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,14 +894,13 @@
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,10 +911,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>12</v>
@@ -917,11 +922,8 @@
       <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -931,23 +933,20 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>3.6669999999999998</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>0.78</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>0.20100000000000001</v>
       </c>
-      <c r="H2" s="1">
-        <v>7.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -957,23 +956,20 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>2.6349999999999998</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>0.73699999999999999</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>0.86099999999999999</v>
       </c>
-      <c r="H3" s="1">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -983,23 +979,20 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1009,23 +1002,20 @@
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>0.123</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>1.883</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>0.94799999999999995</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>0.66100000000000003</v>
       </c>
-      <c r="H5" s="1">
-        <v>0.21099999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1035,23 +1025,20 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>1.5369999999999999</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>0.54900000000000004</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>2E-3</v>
       </c>
-      <c r="H6" s="1">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1061,23 +1048,20 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>0.45100000000000001</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>0.39</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>0.248</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H7" s="1">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1087,23 +1071,20 @@
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1">
-        <v>1.163</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.78900000000000003</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.752</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.93100000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>0.183</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.17</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.876</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.32200000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1113,23 +1094,20 @@
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1">
-        <v>1.3260000000000001</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.4E-2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0.19900000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.80200000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1139,23 +1117,20 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>1.3720000000000001</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>0.76100000000000001</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>0.68400000000000005</v>
       </c>
-      <c r="H10" s="1">
-        <v>0.309</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1165,23 +1140,20 @@
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>0.88300000000000001</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>0.54400000000000004</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>0.104</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>0.81399999999999995</v>
       </c>
-      <c r="H11" s="1">
-        <v>0.33900000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1191,23 +1163,20 @@
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1">
-        <v>1.0609999999999999</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.25900000000000001</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.628</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.35399999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>-0.44700000000000001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.4690000000000001</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.19800000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1217,23 +1186,20 @@
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="1">
-        <v>1.2410000000000001</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1.0640000000000001</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.3660000000000001</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.20100000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1243,23 +1209,20 @@
       <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>0.13700000000000001</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>1.22</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="3">
         <v>0.91100000000000003</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>0.79700000000000004</v>
       </c>
-      <c r="H14" s="1">
-        <v>0.63600000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1269,23 +1232,21 @@
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <v>1.2949999999999999</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>0.71399999999999997</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>0.93</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0.70399999999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>